<commit_message>
new sample report and export format
</commit_message>
<xml_diff>
--- a/docs/sample_report.xlsx
+++ b/docs/sample_report.xlsx
@@ -448,7 +448,7 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
@@ -456,11 +456,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="31" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="50" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="31" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
     <col width="23" customWidth="1" min="7" max="7"/>
     <col width="25" customWidth="1" min="8" max="8"/>
@@ -484,27 +484,27 @@
     <row r="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Channel__c</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Id</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -601,27 +601,27 @@
     <row r="2" ht="15" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
+          <t>7012H000000seXoQAI</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Saasquatch_Verbal_USCA</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Referrals</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Email Only</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Referral</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>7012H000000seXoQAI</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -683,32 +683,32 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Prospect likely engaged with the Saasquatch_Verbal_USCA campaign through a warm introduction or trusted verbal referral, indicating high interest and intent. This suggests they are in the consideration stage of the buyer's journey.</t>
+          <t>Prospects engaged via high-trust verbal referrals for Saasquatch in the US. Likely interested due to trusted recommendations, indicating strong intent and high readiness to explore solutions. Shows they are actively seeking solutions, likely in the con...</t>
         </is>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
+          <t>7012H000001gtUFQAY</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Digital_Invoca_WalkOn</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Walk-On</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>7012H000001gtUFQAY</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
           <t>Walk-On</t>
@@ -762,34 +762,34 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>Prospect initiated contact directly from US, showing high interest and possible urgency. Their intent suggests active research or immediate need, indicating they are likely in the consideration or decision stage.</t>
+          <t>Prospect likely engaged with Digital_Invoca_WalkOn campaign by self-submitting an inquiry, showing high initiative and potential urgency. Direct engagement indicates strong interest, possibly in urgent need. Indicates mid-to-late buyer's journey stage.</t>
         </is>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" t="inlineStr">
         <is>
+          <t>7012H000001hVwqQAE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>Google_US_Search_Brand_Exact</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Paid Search</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Advertisement</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Brand_Exact</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>7012H000001hVwqQAE</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -877,34 +877,34 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>Prospects actively searching for communication solutions clicked on search ads, showing high intent for UCaaS. Likely IT decision makers at small businesses seeking cost-effective, scalable options. In the consideration stage of the buyer's journey.</t>
+          <t>Prospects actively seeking communication solutions clicked on Google search ads for RingCentral, indicating high intent for UCaaS. Likely IT decision-makers in small businesses, aiming for cost savings and growth, showing late-stage buyer journey inter...</t>
         </is>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" t="inlineStr">
         <is>
+          <t>7012H000001hVwrQAE</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>Google_US_Search_Brand_Phrase</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Paid Search</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Advertisement</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Brand_Phrase</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>7012H000001hVwrQAE</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -992,34 +992,34 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>Prospects actively searching for communication solutions, likely IT decision makers for unified communications, showing high intent and brand awareness. Indicates mid to late-stage buyer's journey for small businesses scaling operations.</t>
+          <t>Prospects actively seeking communication solutions, especially UCaaS/business phone systems, showing high IT decision-making interest. Likely in consideration stage of buyer's journey, looking for cost-effective, scalable options for small businesses.</t>
         </is>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" t="inlineStr">
         <is>
+          <t>7012H000001hVx3QAE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>Google_US_Search_Fax_Exact</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Paid Search</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Advertisement</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Fax_Exact</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>7012H000001hVx3QAE</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>Prospects actively searching for communication solutions, comparing options for business phone systems. Likely IT decision makers at small businesses focused on fast setup and growth. Early to mid-buyer's journey stage.</t>
+          <t>Prospects actively searching for communication solutions, likely comparing options for a business phone system. Indicates mid-stage buyer's journey for a small business IT decision maker considering UCaaS.</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>229.6 chars</t>
+          <t>243.6 chars</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-07-14 11:44:54</t>
+          <t>2025-07-14 12:13:22</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
new sample report over 50 campaign members (14 campaign descriptions enhanced)
</commit_message>
<xml_diff>
--- a/docs/sample_report.xlsx
+++ b/docs/sample_report.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
@@ -457,18 +457,18 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="31" customWidth="1" min="2" max="2"/>
-    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="38" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="50" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="19" customWidth="1" min="6" max="6"/>
     <col width="23" customWidth="1" min="7" max="7"/>
     <col width="25" customWidth="1" min="8" max="8"/>
     <col width="21" customWidth="1" min="9" max="9"/>
     <col width="32" customWidth="1" min="10" max="10"/>
     <col width="16" customWidth="1" min="11" max="11"/>
-    <col width="14" customWidth="1" min="12" max="12"/>
-    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="24" customWidth="1" min="12" max="12"/>
+    <col width="36" customWidth="1" min="13" max="13"/>
     <col width="13" customWidth="1" min="14" max="14"/>
     <col width="36" customWidth="1" min="15" max="15"/>
     <col width="14" customWidth="1" min="16" max="16"/>
@@ -683,7 +683,7 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Prospects engaged via high-trust verbal referrals for Saasquatch in the US. Likely interested due to trusted recommendations, indicating strong intent and high readiness to explore solutions. Shows they are actively seeking solutions, likely in the con...</t>
+          <t>Prospects were referred to Saasquatch via a trusted source, likely indicating strong interest or need. Their engagement suggests they are in the consideration stage of the buyer's journey.</t>
         </is>
       </c>
     </row>
@@ -762,7 +762,7 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>Prospect likely engaged with Digital_Invoca_WalkOn campaign by self-submitting an inquiry, showing high initiative and potential urgency. Direct engagement indicates strong interest, possibly in urgent need. Indicates mid-to-late buyer's journey stage.</t>
+          <t>Prospect self-submitted, likely urgently needing Invoca's digital solution. Directly found us. Engaged with generic email, showing high initiative. In early to mid-buyer's journey stage.</t>
         </is>
       </c>
     </row>
@@ -877,7 +877,7 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>Prospects actively seeking communication solutions clicked on Google search ads for RingCentral, indicating high intent for UCaaS. Likely IT decision-makers in small businesses, aiming for cost savings and growth, showing late-stage buyer journey inter...</t>
+          <t>Prospects actively searching for communication solutions with high intent found via RingCentral brand search, indicating IT decision makers in small businesses scaling up, likely in the consideration stage of the buyer's journey.</t>
         </is>
       </c>
     </row>
@@ -992,7 +992,7 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>Prospects actively seeking communication solutions, especially UCaaS/business phone systems, showing high IT decision-making interest. Likely in consideration stage of buyer's journey, looking for cost-effective, scalable options for small businesses.</t>
+          <t>Prospect actively searched for communication solutions, focusing on RingCentral, showing high intent as a small business IT decision maker exploring UCaaS. Likely in the consideration stage of their buyer's journey.</t>
         </is>
       </c>
     </row>
@@ -1107,7 +1107,838 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>Prospects actively searching for communication solutions, likely comparing options for a business phone system. Indicates mid-stage buyer's journey for a small business IT decision maker considering UCaaS.</t>
+          <t>Prospects actively searching for communication solutions, likely comparing options for a business phone system. Indicates mid-funnel buyer considering IT decisions for unified communications.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>7012H000001hVx6QAE</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Google_US_Search_Phone_Systems_Exact</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Paid Search</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Advertisement</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Phone_Systems_Exact</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Search Engines</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>SEM - Non-Brand</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>MVP/PBX to Cloud</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>RingEX</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Hello to Growing Your Business</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Google</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Easily set up and grow my business</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="R7" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Phone_Systems_Exact</t>
+        </is>
+      </c>
+      <c r="U7" t="n">
+        <v>1</v>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
+            1. What the prospect was doing when they engaged with this campaign
+            2. Why they likely engaged (their intent/interest)
+            3. What this tells us about their buyer's journey stage
+            Focus on the prospect's perspective and intent, not marketing terminology.
+            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+            Campaign Information:
+            Campaign: Google_US_Search_Phone_Systems_Exact
+Engagement method: Clicked on search ads - actively searching for communication solutions with high intent
+Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
+Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: SEM/SEO driven - paid or organic search
+Specific engagement context: Searched generic terms like 'business phone system' - comparing solutions
+Target customer profile campaign identifier: Small business scaling - fast setup, flexible usage, and business growth
+Campaign format: Ad campaign response - varying intent based on ad type
+Lead source context: Google Ads - paid search intent
+Value proposition focus: SMB messaging - simplicity and growth focus
+Campaign description: Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Phone_Systems_Exact
+Campaign title: Google_US_Search_Phone_Systems_Exact
+Target geographic market for campaign: US
+Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
+Concise sales focused campaign summary: Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Phone_Systems_Exact
+            Description (max 255 characters):</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>Prospects actively searching for business phone systems on Google US likely seek cost-effective UCaaS solutions. They are comparing options, indicating mid to late buyer's journey stage as small businesses scaling up.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7012H000001l35sQAA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Affiliates_TheTop10sites</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Affiliates</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Prospect visited RingCentral Office Landing Page from a Comparison/Review Website - TheTop10Sites.com (https://www.thetop10sites.com/business-voip/) and submitted their info through the web form or called in.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Direct Affiliates</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Affiliates - CPL</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>MVP/PBX to Cloud</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>RingEX</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Greenfield</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>RingEX SMB Acquisition</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Better Impression (US)</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="R8" t="b">
+        <v>0</v>
+      </c>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Prospect visited RingCentral Office Landing Page from a Comparison/Review Website - TheTop10Sites.com (https://www.thetop10sites.com/business-voip/) and submitted their info through the web form or called in.</t>
+        </is>
+      </c>
+      <c r="U8" t="n">
+        <v>1</v>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
+            1. What the prospect was doing when they engaged with this campaign
+            2. Why they likely engaged (their intent/interest)
+            3. What this tells us about their buyer's journey stage
+            Focus on the prospect's perspective and intent, not marketing terminology.
+            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+            Campaign Information:
+            Campaign: Affiliates_TheTop10sites
+Engagement method: Referred through affiliate partner - has some context about RingCentral
+Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
+Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: Referred by direct affiliate - warm intro with initial context
+Specific engagement context: Affiliate referral - cost-per-lead, mid-intent form fill
+Target customer profile program classification: Ongoing evergreen campaign - continous lead flow
+Target customer profile and strategy: Targeting small business (1-499 employees) - faster sales cycle, price sensitive
+Lead source context: Better Impression (US)
+Company size segment: 20-99 employees - growing company, scalability important
+Buyer journey stage: High intent - actively evaluating solutions (demo, trial, pricing interest)
+Campaign description: Prospect visited RingCentral Office Landing Page from a Comparison/Review Website - TheTop10Sites.com (https://www.thetop10sites.com/business-voip/) and submitted their info through the web form or called in.
+Campaign title: Affiliates_TheTop10sites
+Target geographic market for campaign: US
+Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
+Concise sales focused campaign summary: Prospect visited RingCentral Office Landing Page from a Comparison/Review Website - TheTop10Sites.com (https://www.thetop10sites.com/business-voip/) and submitted their info through the web form or called in.
+            Description (max 255 characters):</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>Prospect researching business phone systems on TheTop10Sites.com followed a cost-saving lead to RingCentral. High-intent evaluation stage, likely IT decision maker.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>7012H000001l3BBQAY</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Affiliates_BusinessBPS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Affiliates</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Prospect visited RingCentral Office Landing Page from a Content/Review Website - Business.com (https://www.business.com/categories/business-phone-systems/) and submitted their info through the web form or called in.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Direct Affiliates</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Affiliates - CPC</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>MVP/PBX to Cloud</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>RingEX</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Greenfield</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>RingEX SMB Acquisition</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Purch (Business News Daily - VOIP)</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="R9" t="b">
+        <v>0</v>
+      </c>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Prospect visited RingCentral Office Landing Page from a Content/Review Website - Business.com (https://www.business.com/categories/business-phone-systems/) and submitted their info through the web form or called in.</t>
+        </is>
+      </c>
+      <c r="U9" t="n">
+        <v>1</v>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
+            1. What the prospect was doing when they engaged with this campaign
+            2. Why they likely engaged (their intent/interest)
+            3. What this tells us about their buyer's journey stage
+            Focus on the prospect's perspective and intent, not marketing terminology.
+            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+            Campaign Information:
+            Campaign: Affiliates_BusinessBPS
+Engagement method: Referred through affiliate partner - has some context about RingCentral
+Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
+Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: Referred by direct affiliate - warm intro with initial context
+Specific engagement context: Clicked cost-per-click affiliate link - low-friction awareness
+Target customer profile program classification: Ongoing evergreen campaign - continous lead flow
+Target customer profile and strategy: Targeting small business (1-499 employees) - faster sales cycle, price sensitive
+Lead source context: Purch (Business News Daily - VOIP)
+Company size segment: 20-99 employees - growing company, scalability important
+Buyer journey stage: High intent - actively evaluating solutions (demo, trial, pricing interest)
+Campaign description: Prospect visited RingCentral Office Landing Page from a Content/Review Website - Business.com (https://www.business.com/categories/business-phone-systems/) and submitted their info through the web form or called in.
+Campaign title: Affiliates_BusinessBPS
+Target geographic market for campaign: US
+Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
+Concise sales focused campaign summary: Prospect visited RingCentral Office Landing Page from a Content/Review Website - Business.com (https://www.business.com/categories/business-phone-systems/) and submitted their info through the web form or called in.
+            Description (max 255 characters):</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>Prospect actively seeking unified communications solution for cost savings, likely an IT decision maker. High-intent evaluation stage, engaging through low-friction affiliate link from Business.com.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>70134000001CjkkAAC</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Bing_US_Search_Brand_Exact</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Paid Search</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Paid Search</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Brand Search</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>SEM - Brand</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>RingEX</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Bing</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="R10" t="b">
+        <v>0</v>
+      </c>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Paid Search</t>
+        </is>
+      </c>
+      <c r="U10" t="n">
+        <v>1</v>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
+            1. What the prospect was doing when they engaged with this campaign
+            2. Why they likely engaged (their intent/interest)
+            3. What this tells us about their buyer's journey stage
+            Focus on the prospect's perspective and intent, not marketing terminology.
+            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+            Campaign Information:
+            Campaign: Bing_US_Search_Brand_Exact
+Engagement method: Clicked on search ads - actively searching for communication solutions with high intent
+Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: Found via RingCentral brand keyword search - direct high intent query
+Specific engagement context: Searched 'RingCentral' or product names - brand aware, high intent
+Lead source context: Bing
+Campaign description: Paid Search
+Campaign title: Bing_US_Search_Brand_Exact
+Target geographic market for campaign: US
+Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
+Concise sales focused campaign summary: Paid Search
+            Description (max 255 characters):</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>Prospects actively searching for communication solutions clicked on Bing search ads for 'RingCentral' or related terms, showing high intent. Likely IT decision makers in the buying stage evaluating UCaaS options.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>70134000001XyCZAA0</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RCO/ACO_Price_Parity</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>VAR MDF</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Events</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>RingEX</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>VAR Marketing</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="R11" t="b">
+        <v>0</v>
+      </c>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="n">
+        <v>1</v>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
+            1. What the prospect was doing when they engaged with this campaign
+            2. Why they likely engaged (their intent/interest)
+            3. What this tells us about their buyer's journey stage
+            Focus on the prospect's perspective and intent, not marketing terminology.
+            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+            Campaign Information:
+            Campaign: RCO/ACO_Price_Parity
+Engagement method: Campaign funded through reseller marketing - likely co-branded outreach via trusted tech advisor
+Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: Event marketing - webinars, conferences, tradeshows
+Lead source context: VAR Marketing
+Campaign title: RCO/ACO_Price_Parity
+Target geographic market for campaign: US
+Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
+            Description (max 255 characters):</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>Prospects engaged with the RCO/ACO_Price_Parity campaign, seeking price parity for UCaaS solutions. Likely IT decision makers exploring unified communications options, indicating a mid-stage buyer's journey.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>70180000000OwaeAAC</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SEO_GoogleRC</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Organic Search</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Search Engines</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>RingEX</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="R12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="n">
+        <v>5</v>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
+            1. What the prospect was doing when they engaged with this campaign
+            2. Why they likely engaged (their intent/interest)
+            3. What this tells us about their buyer's journey stage
+            Focus on the prospect's perspective and intent, not marketing terminology.
+            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+            Campaign Information:
+            Campaign: SEO_GoogleRC
+Engagement method: Found us through organic search - self-directed research, comparing options
+Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: SEM/SEO driven - paid or organic search
+Campaign title: SEO_GoogleRC
+Target geographic market for campaign: US
+Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
+            Description (max 255 characters):</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>Prospects conducting self-research on Google for UCaaS options in the US found us through SEO_GoogleRC. Likely IT decision makers at the comparison stage of their buyer's journey.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>701800000019F0iAAE</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Sales Generated</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Walk-On</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Sales Generated</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="R13" t="b">
+        <v>0</v>
+      </c>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="n">
+        <v>21</v>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
+            1. What the prospect was doing when they engaged with this campaign
+            2. Why they likely engaged (their intent/interest)
+            3. What this tells us about their buyer's journey stage
+            Focus on the prospect's perspective and intent, not marketing terminology.
+            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+            Campaign Information:
+            Campaign: Sales Generated
+Engagement method: Self-submitted or inbound lead without campaign - high initiative, potentially urgent need
+Secondary channel: Entered by sales team from internal source - low initial engagement
+Campaign title: Sales Generated
+Target geographic market for campaign: US
+Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
+            Description (max 255 characters):</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>Prospects likely sought help urgently when engaging with "Sales Generated" campaign from the US. Their high initiative suggests immediate needs, placing them in the decision-making stage of the buyer's journey.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>701Hr000000t6JrIAI</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>HealthcareLPformfills</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Healthcare integrated campaign</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>website</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Healthcare</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Healthcare</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="R14" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Healthcare integrated campaign</t>
+        </is>
+      </c>
+      <c r="U14" t="n">
+        <v>1</v>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
+            1. What the prospect was doing when they engaged with this campaign
+            2. Why they likely engaged (their intent/interest)
+            3. What this tells us about their buyer's journey stage
+            Focus on the prospect's perspective and intent, not marketing terminology.
+            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+            Campaign Information:
+            Campaign: HealthcareLPformfills
+Engagement method: Engagment channel not categorized - review needed to determine buyer intent
+Secondary channel: Direct website visit or form fill - proactive buyer behavior
+Lead source context: Healthcare
+Industry context: Healthcare industry - HIPAA compilance needs
+Campaign description: Healthcare integrated campaign
+Campaign title: HealthcareLPformfills
+Target geographic market for campaign: US
+Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
+Concise sales focused campaign summary: Healthcare integrated campaign
+            Description (max 255 characters):</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>Prospects actively sought healthcare solutions via direct website visits or form fills, showing proactive interest in HIPAA compliance. Indicates mid to late buyer's journey stages.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>701Hr000002I3SJIA0</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>True_Walk_On_2024</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Walk-On</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Walk-On</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="R15" t="b">
+        <v>0</v>
+      </c>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="n">
+        <v>5</v>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
+            1. What the prospect was doing when they engaged with this campaign
+            2. Why they likely engaged (their intent/interest)
+            3. What this tells us about their buyer's journey stage
+            Focus on the prospect's perspective and intent, not marketing terminology.
+            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+            Campaign Information:
+            Campaign: True_Walk_On_2024
+Engagement method: Self-submitted or inbound lead without campaign - high initiative, potentially urgent need
+Secondary channel: Inbound lead without source - prospect found us directly
+Campaign title: True_Walk_On_2024
+Target geographic market for campaign: US
+Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
+            Description (max 255 characters):</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>The prospect proactively sought information about "True_Walk_On_2024," indicating a high initiative and potentially urgent need. They likely engaged due to a direct interest in the campaign topic, showing an advanced stage in their buyer's journey.</t>
         </is>
       </c>
     </row>
@@ -1163,7 +1994,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -1173,7 +2004,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -1206,7 +2037,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>243.6 chars</t>
+          <t>201.8 chars</t>
         </is>
       </c>
     </row>
@@ -1217,7 +2048,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
@@ -1227,7 +2058,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.17</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -1237,7 +2068,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
@@ -1247,7 +2078,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
@@ -1267,7 +2098,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
@@ -1287,7 +2118,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
@@ -1297,7 +2128,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1">
@@ -1308,7 +2139,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-07-14 12:13:22</t>
+          <t>2025-07-14 12:31:06</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
improved prompting lgoic-- tailored prompts based on campaign channel
</commit_message>
<xml_diff>
--- a/docs/sample_report.xlsx
+++ b/docs/sample_report.xlsx
@@ -662,14 +662,10 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: Saasquatch_Verbal_USCA
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. This lead came through a trusted third party referral or partner. 2. What the partnership suggests about product fit or integration potential. 3. How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: Saasquatch_Verbal_USCA
 Engagement method: Customer or partner referral - high trust, warm introduction
 Secondary channel: Direct verbal referral - trusted, high-conversion channel
 Campaign format: Generic email campaign engagment - intent and quality depend on content
@@ -678,12 +674,12 @@
 Campaign title: Saasquatch_Verbal_USCA
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Prospects were referred to Saasquatch via a trusted source, likely indicating strong interest or need. Their engagement suggests they are in the consideration stage of the buyer's journey.</t>
+          <t>Lead from Saasquatch_Verbal_USCA campaign via trusted partner referral signals strong product fit and potential integration with our solutions. Leverage referral trust and emphasize ecosystem relevance in outreach.</t>
         </is>
       </c>
     </row>
@@ -743,26 +739,22 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: Digital_Invoca_WalkOn
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The prospect attended a live event or self submitted interest. 2. What this action suggests about their current interest or goals. 3. How to follow up in a relationship driven or consultative way. Focus on event context and tailoring outreach around shared experience or learning goals.
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: Digital_Invoca_WalkOn
 Engagement method: Self-submitted or inbound lead without campaign - high initiative, potentially urgent need
 Secondary channel: Inbound lead without source - prospect found us directly
 Campaign format: Generic email campaign engagment - intent and quality depend on content
 Campaign title: Digital_Invoca_WalkOn
 Target geographic market for campaign: US
 Attribution tracking: Cannot directly trace leads back to this campaign (lead may have been influenced by campaign)
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>Prospect self-submitted, likely urgently needing Invoca's digital solution. Directly found us. Engaged with generic email, showing high initiative. In early to mid-buyer's journey stage.</t>
+          <t>Prospect engaged with Digital_Invoca_WalkOn, showing high initiative. Likely has urgent needs. Follow up by referencing shared event experience or learning goals from the campaign. Maintain a relationship-driven approach, emphasizing common interests.</t>
         </is>
       </c>
     </row>
@@ -850,14 +842,10 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: Google_US_Search_Brand_Exact
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The lead actively searched for a solution or visited our site. 2. What keyword or campaign may have triggered the engagement. 3. How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: Google_US_Search_Brand_Exact
 Engagement method: Clicked on search ads - actively searching for communication solutions with high intent
 Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
 Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
@@ -872,12 +860,12 @@
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
 Concise sales focused campaign summary: Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Brand_Exact
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>Prospects actively searching for communication solutions with high intent found via RingCentral brand search, indicating IT decision makers in small businesses scaling up, likely in the consideration stage of the buyer's journey.</t>
+          <t>Lead actively searching for communication solutions, likely IT decision maker for UCaaS. Triggered by high-intent 'RingCentral' search. Tailor outreach to highlight cost savings, fast setup, and SMB growth benefits.</t>
         </is>
       </c>
     </row>
@@ -965,14 +953,10 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: Google_US_Search_Brand_Phrase
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The lead actively searched for a solution or visited our site. 2. What keyword or campaign may have triggered the engagement. 3. How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: Google_US_Search_Brand_Phrase
 Engagement method: Clicked on search ads - actively searching for communication solutions with high intent
 Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
 Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
@@ -987,12 +971,12 @@
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
 Concise sales focused campaign summary: Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Brand_Phrase
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>Prospect actively searched for communication solutions, focusing on RingCentral, showing high intent as a small business IT decision maker exploring UCaaS. Likely in the consideration stage of their buyer's journey.</t>
+          <t>Lead actively seeking UCaaS/business phone system solutions via Google search ads. High intent, brand-aware. Tailor outreach with urgency for cost savings pitch, ideal for small businesses scaling rapidly.</t>
         </is>
       </c>
     </row>
@@ -1080,14 +1064,10 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: Google_US_Search_Fax_Exact
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The lead actively searched for a solution or visited our site. 2. What keyword or campaign may have triggered the engagement. 3. How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: Google_US_Search_Fax_Exact
 Engagement method: Clicked on search ads - actively searching for communication solutions with high intent
 Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
 Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
@@ -1102,12 +1082,12 @@
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
 Concise sales focused campaign summary: Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Fax_Exact
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>Prospects actively searching for communication solutions, likely comparing options for a business phone system. Indicates mid-funnel buyer considering IT decisions for unified communications.</t>
+          <t>Lead actively sought communication solutions, likely comparing business phone systems, triggered by 'business phone system' search ads. Tailor outreach with urgency on cost savings, fast setup, and scalability for small businesses.</t>
         </is>
       </c>
     </row>
@@ -1195,14 +1175,10 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: Google_US_Search_Phone_Systems_Exact
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The lead actively searched for a solution or visited our site. 2. What keyword or campaign may have triggered the engagement. 3. How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: Google_US_Search_Phone_Systems_Exact
 Engagement method: Clicked on search ads - actively searching for communication solutions with high intent
 Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
 Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
@@ -1217,12 +1193,12 @@
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
 Concise sales focused campaign summary: Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Phone_Systems_Exact
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>Prospects actively searching for business phone systems on Google US likely seek cost-effective UCaaS solutions. They are comparing options, indicating mid to late buyer's journey stage as small businesses scaling up.</t>
+          <t>Lead actively searched for communication solutions on Google_US_Search_Phone_Systems_Exact, likely triggered by 'business phone system' keywords. Tailor outreach based on urgent need for UCaaS, IT decision maker role, and comparison of solutions for small businesses focusing on simplicity, growth, and cost savings.</t>
         </is>
       </c>
     </row>
@@ -1306,14 +1282,10 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: Affiliates_TheTop10sites
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. This lead came through a trusted third party referral or partner. 2. What the partnership suggests about product fit or integration potential. 3. How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: Affiliates_TheTop10sites
 Engagement method: Referred through affiliate partner - has some context about RingCentral
 Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
 Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
@@ -1329,12 +1301,12 @@
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
 Concise sales focused campaign summary: Prospect visited RingCentral Office Landing Page from a Comparison/Review Website - TheTop10Sites.com (https://www.thetop10sites.com/business-voip/) and submitted their info through the web form or called in.
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>Prospect researching business phone systems on TheTop10Sites.com followed a cost-saving lead to RingCentral. High-intent evaluation stage, likely IT decision maker.</t>
+          <t>Lead from TheTop10Sites.com referral indicates a strong product fit for UCaaS/business phone systems. Leverage this credibility to emphasize integration potential and reach out with confidence.</t>
         </is>
       </c>
     </row>
@@ -1418,14 +1390,10 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: Affiliates_BusinessBPS
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. This lead came through a trusted third party referral or partner. 2. What the partnership suggests about product fit or integration potential. 3. How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: Affiliates_BusinessBPS
 Engagement method: Referred through affiliate partner - has some context about RingCentral
 Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
 Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
@@ -1441,12 +1409,12 @@
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
 Concise sales focused campaign summary: Prospect visited RingCentral Office Landing Page from a Content/Review Website - Business.com (https://www.business.com/categories/business-phone-systems/) and submitted their info through the web form or called in.
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>Prospect actively seeking unified communications solution for cost savings, likely an IT decision maker. High-intent evaluation stage, engaging through low-friction affiliate link from Business.com.</t>
+          <t>Lead referred through trusted affiliate partner, indicating strong fit with RingCentral's UCaaS. Leverage partnership credibility to highlight seamless integration potential in outreach.</t>
         </is>
       </c>
     </row>
@@ -1518,14 +1486,10 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: Bing_US_Search_Brand_Exact
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The lead actively searched for a solution or visited our site. 2. What keyword or campaign may have triggered the engagement. 3. How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: Bing_US_Search_Brand_Exact
 Engagement method: Clicked on search ads - actively searching for communication solutions with high intent
 Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
 Secondary channel: Found via RingCentral brand keyword search - direct high intent query
@@ -1536,12 +1500,12 @@
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
 Concise sales focused campaign summary: Paid Search
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>Prospects actively searching for communication solutions clicked on Bing search ads for 'RingCentral' or related terms, showing high intent. Likely IT decision makers in the buying stage evaluating UCaaS options.</t>
+          <t>Lead actively searched for communication solutions, likely an IT decision maker interested in UCaaS/business phone systems. Triggered by brand keyword 'RingCentral'. Tailor outreach by emphasizing urgency for solution comparison.</t>
         </is>
       </c>
     </row>
@@ -1601,14 +1565,10 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: RCO/ACO_Price_Parity
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. This lead came through a trusted third party referral or partner. 2. What the partnership suggests about product fit or integration potential. 3. How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: RCO/ACO_Price_Parity
 Engagement method: Campaign funded through reseller marketing - likely co-branded outreach via trusted tech advisor
 Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
 Secondary channel: Event marketing - webinars, conferences, tradeshows
@@ -1616,12 +1576,12 @@
 Campaign title: RCO/ACO_Price_Parity
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>Prospects engaged with the RCO/ACO_Price_Parity campaign, seeking price parity for UCaaS solutions. Likely IT decision makers exploring unified communications options, indicating a mid-stage buyer's journey.</t>
+          <t>Lead acquired via trusted VAR marketing campaign with tech advisor, indicating strong fit for UCaaS integration. Leverage referral trust &amp; ecosystem relevance to guide outreach.</t>
         </is>
       </c>
     </row>
@@ -1677,26 +1637,22 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: SEO_GoogleRC
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The lead actively searched for a solution or visited our site. 2. What keyword or campaign may have triggered the engagement. 3. How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: SEO_GoogleRC
 Engagement method: Found us through organic search - self-directed research, comparing options
 Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
 Secondary channel: SEM/SEO driven - paid or organic search
 Campaign title: SEO_GoogleRC
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>Prospects conducting self-research on Google for UCaaS options in the US found us through SEO_GoogleRC. Likely IT decision makers at the comparison stage of their buyer's journey.</t>
+          <t>Lead actively researched UCaaS solutions on Google, likely comparing options. Tailor outreach to highlight urgency, readiness, and our solution fit for IT decision makers. Campaign likely triggered by SEO_GoogleRC.</t>
         </is>
       </c>
     </row>
@@ -1752,25 +1708,21 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: Sales Generated
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The prospect attended a live event or self submitted interest. 2. What this action suggests about their current interest or goals. 3. How to follow up in a relationship driven or consultative way. Focus on event context and tailoring outreach around shared experience or learning goals.
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: Sales Generated
 Engagement method: Self-submitted or inbound lead without campaign - high initiative, potentially urgent need
 Secondary channel: Entered by sales team from internal source - low initial engagement
 Campaign title: Sales Generated
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>Prospects likely sought help urgently when engaging with "Sales Generated" campaign from the US. Their high initiative suggests immediate needs, placing them in the decision-making stage of the buyer's journey.</t>
+          <t>Prospect attended a live event or self-submitted interest with high initiative, indicating an urgent need. Follow up with a consultative approach, referencing shared learning goals from the event or website domain experience.</t>
         </is>
       </c>
     </row>
@@ -1842,14 +1794,10 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: HealthcareLPformfills
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. This is a sales-sourced contact (not from prospect engagement). 2. The data source and why this contact was identified. 3. What approach might work best for cold outreach. Focus on the sales context and potential fit, not prospect behavior (since they haven't engaged).
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: HealthcareLPformfills
 Engagement method: Engagment channel not categorized - review needed to determine buyer intent
 Secondary channel: Direct website visit or form fill - proactive buyer behavior
 Lead source context: Healthcare
@@ -1859,12 +1807,12 @@
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
 Concise sales focused campaign summary: Healthcare integrated campaign
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>Prospects actively sought healthcare solutions via direct website visits or form fills, showing proactive interest in HIPAA compliance. Indicates mid to late buyer's journey stages.</t>
+          <t>Sales-sourced contact from HealthcareLPformfills campaign. Identified through proactive form fill on healthcare website. Best approach: Highlight HIPAA compliance fit in US market for cold outreach.</t>
         </is>
       </c>
     </row>
@@ -1920,25 +1868,21 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand:
-            1. What the prospect was doing when they engaged with this campaign
-            2. Why they likely engaged (their intent/interest)
-            3. What this tells us about their buyer's journey stage
-            Focus on the prospect's perspective and intent, not marketing terminology.
-            IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
-            Campaign Information:
-            Campaign: True_Walk_On_2024
+          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The prospect attended a live event or self submitted interest. 2. What this action suggests about their current interest or goals. 3. How to follow up in a relationship driven or consultative way. Focus on event context and tailoring outreach around shared experience or learning goals.
+IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
+Campaign Information:
+Campaign: True_Walk_On_2024
 Engagement method: Self-submitted or inbound lead without campaign - high initiative, potentially urgent need
 Secondary channel: Inbound lead without source - prospect found us directly
 Campaign title: True_Walk_On_2024
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
-            Description (max 255 characters):</t>
+Description (max 255 characters):</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>The prospect proactively sought information about "True_Walk_On_2024," indicating a high initiative and potentially urgent need. They likely engaged due to a direct interest in the campaign topic, showing an advanced stage in their buyer's journey.</t>
+          <t>Prospect engaged with True_Walk_On_2024 event or self-submitted interest, indicating high initiative &amp; possibly urgent need. Follow up by referencing shared learning goals or experiences from the event/domain.com for a consultative approach.</t>
         </is>
       </c>
     </row>
@@ -2037,7 +1981,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>201.8 chars</t>
+          <t>221.1 chars</t>
         </is>
       </c>
     </row>
@@ -2058,7 +2002,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.35</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -2139,7 +2083,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-07-14 12:31:06</t>
+          <t>2025-07-14 14:01:58</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
new sample reports + better prompting logic (targetted and labelled categories for bullet points)
</commit_message>
<xml_diff>
--- a/docs/sample_report.xlsx
+++ b/docs/sample_report.xlsx
@@ -662,7 +662,7 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. This lead came through a trusted third party referral or partner. 2. What the partnership suggests about product fit or integration potential. 3. How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Referral Source: This lead came through a trusted third party referral or partner. • Fit/Alignment: What the partnership suggests about product fit or integration potential. • Leverage: How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Saasquatch_Verbal_USCA
@@ -679,7 +679,9 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Lead from Saasquatch_Verbal_USCA campaign via trusted partner referral signals strong product fit and potential integration with our solutions. Leverage referral trust and emphasize ecosystem relevance in outreach.</t>
+          <t>• Referral Source: Trusted third-party referral or partner (Saasquatch).
+• Fit/Alignment: Partnership implies strong product fit or integration potential.
+• Leverage: Utilize referral trust to highlight integration relevance and credibility.</t>
         </is>
       </c>
     </row>
@@ -739,7 +741,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The prospect attended a live event or self submitted interest. 2. What this action suggests about their current interest or goals. 3. How to follow up in a relationship driven or consultative way. Focus on event context and tailoring outreach around shared experience or learning goals.
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Participation: The prospect attended a live event or self submitted interest. • Signal: What this action suggests about their current interest or goals. • Engagement Style: How to follow up in a relationship driven or consultative way. Focus on event context and tailoring outreach around shared experience or learning goals.
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Digital_Invoca_WalkOn
@@ -754,7 +756,9 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>Prospect engaged with Digital_Invoca_WalkOn, showing high initiative. Likely has urgent needs. Follow up by referencing shared event experience or learning goals from the campaign. Maintain a relationship-driven approach, emphasizing common interests.</t>
+          <t>• Participation: Prospect attended Digital_Invoca_WalkOn event.
+• Signal: Strong interest in digital solutions &amp; marketing strategies.
+• Engagement Style: Approach with tailored insights from the event, focus on mutual learning goals and shared experiences.</t>
         </is>
       </c>
     </row>
@@ -842,7 +846,7 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The lead actively searched for a solution or visited our site. 2. What keyword or campaign may have triggered the engagement. 3. How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Search Behavior: The lead actively searched for a solution or visited our site. • Trigger: What keyword or campaign may have triggered the engagement. • Urgency: How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Google_US_Search_Brand_Exact
@@ -865,7 +869,9 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>Lead actively searching for communication solutions, likely IT decision maker for UCaaS. Triggered by high-intent 'RingCentral' search. Tailor outreach to highlight cost savings, fast setup, and SMB growth benefits.</t>
+          <t>• Search Behavior: Lead actively searched for communication solutions, visited RingCentral site.
+• Trigger: Engaged via 'RingCentral' or product-related searches, high intent.
+• Urgency: Tailor outreach on UCaaS benefits for small businesses, stress simplicity and growth.</t>
         </is>
       </c>
     </row>
@@ -953,7 +959,7 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The lead actively searched for a solution or visited our site. 2. What keyword or campaign may have triggered the engagement. 3. How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Search Behavior: The lead actively searched for a solution or visited our site. • Trigger: What keyword or campaign may have triggered the engagement. • Urgency: How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Google_US_Search_Brand_Phrase
@@ -976,7 +982,9 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>Lead actively seeking UCaaS/business phone system solutions via Google search ads. High intent, brand-aware. Tailor outreach with urgency for cost savings pitch, ideal for small businesses scaling rapidly.</t>
+          <t>• Search Behavior: Lead actively searched for communication solutions, likely visited RingCentral site
+• Trigger: Engaged through 'RingCentral' or product name search, indicating high intent
+• Urgency: Tailor outreach for IT decision maker, highlight cost savings, fast setup, growth benefits</t>
         </is>
       </c>
     </row>
@@ -1064,7 +1072,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The lead actively searched for a solution or visited our site. 2. What keyword or campaign may have triggered the engagement. 3. How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Search Behavior: The lead actively searched for a solution or visited our site. • Trigger: What keyword or campaign may have triggered the engagement. • Urgency: How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Google_US_Search_Fax_Exact
@@ -1087,7 +1095,9 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>Lead actively sought communication solutions, likely comparing business phone systems, triggered by 'business phone system' search ads. Tailor outreach with urgency on cost savings, fast setup, and scalability for small businesses.</t>
+          <t>• Search Behavior: Lead actively searched for communication solutions like 'business phone system'.
+• Trigger: Paid search campaign targeting small businesses interested in UCaaS.
+• Urgency: Tailor outreach focusing on fast setup, flexibility, cost savings, and growth opportunities.</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1185,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The lead actively searched for a solution or visited our site. 2. What keyword or campaign may have triggered the engagement. 3. How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Search Behavior: The lead actively searched for a solution or visited our site. • Trigger: What keyword or campaign may have triggered the engagement. • Urgency: How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Google_US_Search_Phone_Systems_Exact
@@ -1198,7 +1208,9 @@
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>Lead actively searched for communication solutions on Google_US_Search_Phone_Systems_Exact, likely triggered by 'business phone system' keywords. Tailor outreach based on urgent need for UCaaS, IT decision maker role, and comparison of solutions for small businesses focusing on simplicity, growth, and cost savings.</t>
+          <t>• Search Behavior: Lead actively searching for communication solutions, likely visited our site.
+• Trigger: Searched 'business phone system' - intent triggered by cost savings pitch.
+• Urgency: Tailor outreach focusing on fast setup, flexibility, and SMB growth needs.</t>
         </is>
       </c>
     </row>
@@ -1282,7 +1294,7 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. This lead came through a trusted third party referral or partner. 2. What the partnership suggests about product fit or integration potential. 3. How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Referral Source: This lead came through a trusted third party referral or partner. • Fit/Alignment: What the partnership suggests about product fit or integration potential. • Leverage: How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Affiliates_TheTop10sites
@@ -1306,7 +1318,9 @@
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>Lead from TheTop10Sites.com referral indicates a strong product fit for UCaaS/business phone systems. Leverage this credibility to emphasize integration potential and reach out with confidence.</t>
+          <t>• Referral Source: Trusted third-party referral from TheTop10Sites.com
+• Fit/Alignment: Implies strong product fit for UCaaS/business phone system
+• Leverage: Highlight partnership credibility, emphasize integration potential</t>
         </is>
       </c>
     </row>
@@ -1390,7 +1404,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. This lead came through a trusted third party referral or partner. 2. What the partnership suggests about product fit or integration potential. 3. How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Referral Source: This lead came through a trusted third party referral or partner. • Fit/Alignment: What the partnership suggests about product fit or integration potential. • Leverage: How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Affiliates_BusinessBPS
@@ -1414,7 +1428,9 @@
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>Lead referred through trusted affiliate partner, indicating strong fit with RingCentral's UCaaS. Leverage partnership credibility to highlight seamless integration potential in outreach.</t>
+          <t>• Referral Source: Referred through trusted partner.
+• Fit/Alignment: Partnership indicates strong product fit.
+• Leverage: Highlight integration relevance, mention referral credibility.</t>
         </is>
       </c>
     </row>
@@ -1486,7 +1502,7 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The lead actively searched for a solution or visited our site. 2. What keyword or campaign may have triggered the engagement. 3. How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Search Behavior: The lead actively searched for a solution or visited our site. • Trigger: What keyword or campaign may have triggered the engagement. • Urgency: How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Bing_US_Search_Brand_Exact
@@ -1505,7 +1521,9 @@
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>Lead actively searched for communication solutions, likely an IT decision maker interested in UCaaS/business phone systems. Triggered by brand keyword 'RingCentral'. Tailor outreach by emphasizing urgency for solution comparison.</t>
+          <t>• Search Behavior: Lead actively searched for communication solutions, visited RingCentral site
+• Trigger: Bing_US_Search_Brand_Exact campaign, RingCentral brand keyword search
+• Urgency: Tailor outreach for IT decision maker, high intent, compare solutions, emphasize UCaaS benefits</t>
         </is>
       </c>
     </row>
@@ -1565,7 +1583,7 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. This lead came through a trusted third party referral or partner. 2. What the partnership suggests about product fit or integration potential. 3. How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Referral Source: This lead came through a trusted third party referral or partner. • Fit/Alignment: What the partnership suggests about product fit or integration potential. • Leverage: How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: RCO/ACO_Price_Parity
@@ -1581,7 +1599,9 @@
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>Lead acquired via trusted VAR marketing campaign with tech advisor, indicating strong fit for UCaaS integration. Leverage referral trust &amp; ecosystem relevance to guide outreach.</t>
+          <t>• Referral Source: Lead from trusted tech advisor
+• Fit/Alignment: Indicates strong fit for UCaaS solutions
+• Leverage: Highlight partnership credibility, emphasize integration potential for unified communications.</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1657,7 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The lead actively searched for a solution or visited our site. 2. What keyword or campaign may have triggered the engagement. 3. How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Search Behavior: The lead actively searched for a solution or visited our site. • Trigger: What keyword or campaign may have triggered the engagement. • Urgency: How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: SEO_GoogleRC
@@ -1652,7 +1672,9 @@
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>Lead actively researched UCaaS solutions on Google, likely comparing options. Tailor outreach to highlight urgency, readiness, and our solution fit for IT decision makers. Campaign likely triggered by SEO_GoogleRC.</t>
+          <t>• Search Behavior: Lead actively researching UCaaS options, found us through organic search.
+• Trigger: Likely searched keywords related to UCaaS or business phone systems.
+• Urgency: Tailor outreach based on solution readiness and immediate need for unified communications.</t>
         </is>
       </c>
     </row>
@@ -1708,7 +1730,7 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The prospect attended a live event or self submitted interest. 2. What this action suggests about their current interest or goals. 3. How to follow up in a relationship driven or consultative way. Focus on event context and tailoring outreach around shared experience or learning goals.
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Participation: The prospect attended a live event or self submitted interest. • Signal: What this action suggests about their current interest or goals. • Engagement Style: How to follow up in a relationship driven or consultative way. Focus on event context and tailoring outreach around shared experience or learning goals.
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Sales Generated
@@ -1722,7 +1744,9 @@
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>Prospect attended a live event or self-submitted interest with high initiative, indicating an urgent need. Follow up with a consultative approach, referencing shared learning goals from the event or website domain experience.</t>
+          <t>• Participation: Prospect self-submitted interest for Sales Generated campaign. 
+• Signal: Shows high initiative and potential urgent need for sales solutions. 
+• Engagement Style: Follow up with a consultative approach, referencing shared learning goals from Sales Generated website.</t>
         </is>
       </c>
     </row>
@@ -1794,7 +1818,7 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. This is a sales-sourced contact (not from prospect engagement). 2. The data source and why this contact was identified. 3. What approach might work best for cold outreach. Focus on the sales context and potential fit, not prospect behavior (since they haven't engaged).
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Source: This is a sales-sourced contact (not from prospect engagement). • Data Origin: The data source and why this contact was identified. • Approach: What approach might work best for cold outreach. Focus on the sales context and potential fit, not prospect behavior (since they haven't engaged).
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: HealthcareLPformfills
@@ -1812,7 +1836,9 @@
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>Sales-sourced contact from HealthcareLPformfills campaign. Identified through proactive form fill on healthcare website. Best approach: Highlight HIPAA compliance fit in US market for cold outreach.</t>
+          <t>• Source: Sales-sourced contact
+• Data Origin: Identified through HealthcareLPformfills campaign
+• Approach: Highlight HIPAA compliance benefits in cold outreach</t>
         </is>
       </c>
     </row>
@@ -1868,7 +1894,7 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, create a concise description (max 255 characters) that helps a salesperson understand: 1. The prospect attended a live event or self submitted interest. 2. What this action suggests about their current interest or goals. 3. How to follow up in a relationship driven or consultative way. Focus on event context and tailoring outreach around shared experience or learning goals.
+          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Participation: The prospect attended a live event or self submitted interest. • Signal: What this action suggests about their current interest or goals. • Engagement Style: How to follow up in a relationship driven or consultative way. Focus on event context and tailoring outreach around shared experience or learning goals.
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: True_Walk_On_2024
@@ -1882,7 +1908,9 @@
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>Prospect engaged with True_Walk_On_2024 event or self-submitted interest, indicating high initiative &amp; possibly urgent need. Follow up by referencing shared learning goals or experiences from the event/domain.com for a consultative approach.</t>
+          <t>• Participation: Prospect self-submitted interest for True_Walk_On_2024.
+• Signal: Indicates high initiative and potentially urgent need.
+• Engagement Style: Emphasize shared experience or learning goals in a consultative follow-up approach.</t>
         </is>
       </c>
     </row>
@@ -1981,7 +2009,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>221.1 chars</t>
+          <t>248.6 chars</t>
         </is>
       </c>
     </row>
@@ -2002,7 +2030,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.42</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -2083,7 +2111,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-07-14 14:01:58</t>
+          <t>2025-07-21 13:55:37</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated conventions + prompting logic
</commit_message>
<xml_diff>
--- a/docs/sample_report.xlsx
+++ b/docs/sample_report.xlsx
@@ -662,13 +662,17 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Referral Source: This lead came through a trusted third party referral or partner. • Fit/Alignment: What the partnership suggests about product fit or integration potential. • Leverage: How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Referral Source: This lead came through a trusted third party referral or partner. 
+• Fit/Alignment: What the partnership suggests about product fit or integration potential. 
+• Leverage: How to use that credibility to guide outreach. 
+Focus on leveraging the referral trust and highlighting integration or ecosystem relevance. 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Saasquatch_Verbal_USCA
-Engagement method: Customer or partner referral - high trust, warm introduction
-Secondary channel: Direct verbal referral - trusted, high-conversion channel
-Campaign format: Generic email campaign engagment - intent and quality depend on content
+Engagement method: Referrals: Customer or partner referral - high trust, warm introduction
+Secondary channel: Verbal Referrals: Direct verbal referral - trusted, high-conversion channel
+Campaign format: Email Only: Generic email campaign engagment - intent and quality depend on content
 Lead source context: Saasquatch
 Campaign description: Referral
 Campaign title: Saasquatch_Verbal_USCA
@@ -679,9 +683,9 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>• Referral Source: Trusted third-party referral or partner (Saasquatch).
-• Fit/Alignment: Partnership implies strong product fit or integration potential.
-• Leverage: Utilize referral trust to highlight integration relevance and credibility.</t>
+          <t>• Referral Source: Lead originated from a trusted partner, indicating high trust and warm introduction.
+• Fit/Alignment: Partnership suggests strong product fit or integration potential with Saasquatch.
+• Leverage: Utilize referral credibility to guide outreach, emphasizing ecosystem relevance and integration possibilities.</t>
         </is>
       </c>
     </row>
@@ -741,13 +745,17 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Participation: The prospect attended a live event or self submitted interest. • Signal: What this action suggests about their current interest or goals. • Engagement Style: How to follow up in a relationship driven or consultative way. Focus on event context and tailoring outreach around shared experience or learning goals.
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Participation: The prospect attended a live event or self submitted interest. 
+• Signal: What this action suggests about their current interest or goals. 
+• Engagement Style: How to follow up in a relationship driven or consultative way. 
+Focus on event context and tailoring outreach around shared experience or learning goals. 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Digital_Invoca_WalkOn
-Engagement method: Self-submitted or inbound lead without campaign - high initiative, potentially urgent need
-Secondary channel: Inbound lead without source - prospect found us directly
-Campaign format: Generic email campaign engagment - intent and quality depend on content
+Engagement method: Walk-On: Self-submitted or inbound lead without campaign - high initiative, potentially urgent need
+Secondary channel: Walk-On: Inbound lead without source - prospect found us directly
+Campaign format: Email: Generic email campaign engagment - intent and quality depend on content
 Campaign title: Digital_Invoca_WalkOn
 Target geographic market for campaign: US
 Attribution tracking: Cannot directly trace leads back to this campaign (lead may have been influenced by campaign)
@@ -756,9 +764,9 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>• Participation: Prospect attended Digital_Invoca_WalkOn event.
-• Signal: Strong interest in digital solutions &amp; marketing strategies.
-• Engagement Style: Approach with tailored insights from the event, focus on mutual learning goals and shared experiences.</t>
+          <t>• Participation: Prospect self-submitted interest or attended an event for Digital Invoca.
+• Signal: Indicates high initiative and potentially urgent need related to Digital Invoca solutions.
+• Engagement Style: Follow up consultatively, highlighting shared learning goals or event experience.</t>
         </is>
       </c>
     </row>
@@ -846,19 +854,23 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Search Behavior: The lead actively searched for a solution or visited our site. • Trigger: What keyword or campaign may have triggered the engagement. • Urgency: How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Search Behavior: The lead actively searched for a solution or visited our site. 
+• Trigger: What keyword or campaign may have triggered the engagement. 
+• Urgency: How to tailor outreach based on urgency or solution comparison. 
+Focus on urgency, buyer readiness, and solution fit. 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Google_US_Search_Brand_Exact
-Engagement method: Clicked on search ads - actively searching for communication solutions with high intent
-Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
-Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
-Secondary channel: Found via RingCentral brand keyword search - direct high intent query
-Specific engagement context: Searched 'RingCentral' or product names - brand aware, high intent
-Target customer profile campaign identifier: Small business scaling - fast setup, flexible usage, and business growth
-Campaign format: Ad campaign response - varying intent based on ad type
-Lead source context: Google Ads - paid search intent
-Value proposition focus: SMB messaging - simplicity and growth focus
+Engagement method: Paid Search: Clicked on search ads - actively searching for communication solutions with high intent
+Cross channel marketing integration indicator: MVP/PBX to Cloud: Migration from on-premise focus - cost savings pitch
+Product interest: RingEX: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: Brand Search: Found via RingCentral brand keyword search - direct high intent query
+Specific engagement context: SEM - Brand: Searched 'RingCentral' or product names - brand aware, high intent
+Target customer profile campaign identifier: Hello to Growing Your Business: Small business scaling - fast setup, flexible usage, and business growth
+Campaign format: Advertisement: Ad campaign response - varying intent based on ad type
+Lead source context: Google: Google Ads - paid search intent
+Value proposition focus: Easily set up and grow my business: SMB messaging - simplicity and growth focus
 Campaign description: Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Brand_Exact
 Campaign title: Google_US_Search_Brand_Exact
 Target geographic market for campaign: US
@@ -869,9 +881,9 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>• Search Behavior: Lead actively searched for communication solutions, visited RingCentral site.
-• Trigger: Engaged via 'RingCentral' or product-related searches, high intent.
-• Urgency: Tailor outreach on UCaaS benefits for small businesses, stress simplicity and growth.</t>
+          <t>• Search Behavior: Lead actively searched for communication solutions, indicating high intent.
+• Trigger: Engaged through 'RingCentral' or related searches, showing brand awareness.
+• Urgency: Tailor outreach for quick setup and growth benefits to meet SMB scaling needs.</t>
         </is>
       </c>
     </row>
@@ -959,19 +971,23 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Search Behavior: The lead actively searched for a solution or visited our site. • Trigger: What keyword or campaign may have triggered the engagement. • Urgency: How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Search Behavior: The lead actively searched for a solution or visited our site. 
+• Trigger: What keyword or campaign may have triggered the engagement. 
+• Urgency: How to tailor outreach based on urgency or solution comparison. 
+Focus on urgency, buyer readiness, and solution fit. 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Google_US_Search_Brand_Phrase
-Engagement method: Clicked on search ads - actively searching for communication solutions with high intent
-Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
-Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
-Secondary channel: Found via RingCentral brand keyword search - direct high intent query
-Specific engagement context: Searched 'RingCentral' or product names - brand aware, high intent
-Target customer profile campaign identifier: Small business scaling - fast setup, flexible usage, and business growth
-Campaign format: Ad campaign response - varying intent based on ad type
-Lead source context: Google Ads - paid search intent
-Value proposition focus: SMB messaging - simplicity and growth focus
+Engagement method: Paid Search: Clicked on search ads - actively searching for communication solutions with high intent
+Cross channel marketing integration indicator: MVP/PBX to Cloud: Migration from on-premise focus - cost savings pitch
+Product interest: RingEX: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: Brand Search: Found via RingCentral brand keyword search - direct high intent query
+Specific engagement context: SEM - Brand: Searched 'RingCentral' or product names - brand aware, high intent
+Target customer profile campaign identifier: Hello to Growing Your Business: Small business scaling - fast setup, flexible usage, and business growth
+Campaign format: Advertisement: Ad campaign response - varying intent based on ad type
+Lead source context: Google: Google Ads - paid search intent
+Value proposition focus: Easily set up and grow my business: SMB messaging - simplicity and growth focus
 Campaign description: Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Brand_Phrase
 Campaign title: Google_US_Search_Brand_Phrase
 Target geographic market for campaign: US
@@ -982,9 +998,9 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>• Search Behavior: Lead actively searched for communication solutions, likely visited RingCentral site
-• Trigger: Engaged through 'RingCentral' or product name search, indicating high intent
-• Urgency: Tailor outreach for IT decision maker, highlight cost savings, fast setup, growth benefits</t>
+          <t>• Search Behavior: Prospect actively searched for communication solutions, likely a small business decision-maker exploring UCaaS options.
+• Trigger: Engaged via Google Ads, indicating high intent for RingCentral's UCaaS solutions.
+• Urgency: Tailor outreach with a focus on fast setup, cost savings, and scalability to meet growing business needs.</t>
         </is>
       </c>
     </row>
@@ -1072,19 +1088,23 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Search Behavior: The lead actively searched for a solution or visited our site. • Trigger: What keyword or campaign may have triggered the engagement. • Urgency: How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Search Behavior: The lead actively searched for a solution or visited our site. 
+• Trigger: What keyword or campaign may have triggered the engagement. 
+• Urgency: How to tailor outreach based on urgency or solution comparison. 
+Focus on urgency, buyer readiness, and solution fit. 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Google_US_Search_Fax_Exact
-Engagement method: Clicked on search ads - actively searching for communication solutions with high intent
-Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
-Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
-Secondary channel: SEM/SEO driven - paid or organic search
-Specific engagement context: Searched generic terms like 'business phone system' - comparing solutions
-Target customer profile campaign identifier: Small business scaling - fast setup, flexible usage, and business growth
-Campaign format: Ad campaign response - varying intent based on ad type
-Lead source context: Google Ads - paid search intent
-Value proposition focus: SMB messaging - simplicity and growth focus
+Engagement method: Paid Search: Clicked on search ads - actively searching for communication solutions with high intent
+Cross channel marketing integration indicator: MVP/PBX to Cloud: Migration from on-premise focus - cost savings pitch
+Product interest: RingEX: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: Search Engines: SEM/SEO driven - paid or organic search
+Specific engagement context: SEM - Non-Brand: Searched generic terms like 'business phone system' - comparing solutions
+Target customer profile campaign identifier: Hello to Growing Your Business: Small business scaling - fast setup, flexible usage, and business growth
+Campaign format: Advertisement: Ad campaign response - varying intent based on ad type
+Lead source context: Google: Google Ads - paid search intent
+Value proposition focus: Easily set up and grow my business: SMB messaging - simplicity and growth focus
 Campaign description: Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Fax_Exact
 Campaign title: Google_US_Search_Fax_Exact
 Target geographic market for campaign: US
@@ -1095,9 +1115,9 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>• Search Behavior: Lead actively searched for communication solutions like 'business phone system'.
-• Trigger: Paid search campaign targeting small businesses interested in UCaaS.
-• Urgency: Tailor outreach focusing on fast setup, flexibility, cost savings, and growth opportunities.</t>
+          <t>• Search Behavior: Prospect actively searched for communication solutions; likely comparing options like business phone systems.
+• Trigger: Engagement possibly triggered by generic terms related to 'business phone system' in SEM non-brand ads.
+• Urgency: Tailor outreach emphasizing RingEX UCaaS fit for IT decision makers seeking cost-effective cloud migration solutions.</t>
         </is>
       </c>
     </row>
@@ -1185,19 +1205,23 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Search Behavior: The lead actively searched for a solution or visited our site. • Trigger: What keyword or campaign may have triggered the engagement. • Urgency: How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Search Behavior: The lead actively searched for a solution or visited our site. 
+• Trigger: What keyword or campaign may have triggered the engagement. 
+• Urgency: How to tailor outreach based on urgency or solution comparison. 
+Focus on urgency, buyer readiness, and solution fit. 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Google_US_Search_Phone_Systems_Exact
-Engagement method: Clicked on search ads - actively searching for communication solutions with high intent
-Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
-Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
-Secondary channel: SEM/SEO driven - paid or organic search
-Specific engagement context: Searched generic terms like 'business phone system' - comparing solutions
-Target customer profile campaign identifier: Small business scaling - fast setup, flexible usage, and business growth
-Campaign format: Ad campaign response - varying intent based on ad type
-Lead source context: Google Ads - paid search intent
-Value proposition focus: SMB messaging - simplicity and growth focus
+Engagement method: Paid Search: Clicked on search ads - actively searching for communication solutions with high intent
+Cross channel marketing integration indicator: MVP/PBX to Cloud: Migration from on-premise focus - cost savings pitch
+Product interest: RingEX: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: Search Engines: SEM/SEO driven - paid or organic search
+Specific engagement context: SEM - Non-Brand: Searched generic terms like 'business phone system' - comparing solutions
+Target customer profile campaign identifier: Hello to Growing Your Business: Small business scaling - fast setup, flexible usage, and business growth
+Campaign format: Advertisement: Ad campaign response - varying intent based on ad type
+Lead source context: Google: Google Ads - paid search intent
+Value proposition focus: Easily set up and grow my business: SMB messaging - simplicity and growth focus
 Campaign description: Paid Search SEM Soiurce - Everygreen Campaign Google_US_Search_Phone_Systems_Exact
 Campaign title: Google_US_Search_Phone_Systems_Exact
 Target geographic market for campaign: US
@@ -1208,9 +1232,9 @@
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>• Search Behavior: Lead actively searching for communication solutions, likely visited our site.
-• Trigger: Searched 'business phone system' - intent triggered by cost savings pitch.
-• Urgency: Tailor outreach focusing on fast setup, flexibility, and SMB growth needs.</t>
+          <t>• Search Behavior: Prospect actively searched for communication solutions, likely comparing options. 
+• Trigger: Engagement possibly triggered by generic terms like 'business phone system.' 
+• Urgency: Tailor outreach with urgency in mind for potential IT decision makers considering RingEX UCaaS.</t>
         </is>
       </c>
     </row>
@@ -1294,19 +1318,23 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Referral Source: This lead came through a trusted third party referral or partner. • Fit/Alignment: What the partnership suggests about product fit or integration potential. • Leverage: How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Referral Source: This lead came through a trusted third party referral or partner. 
+• Fit/Alignment: What the partnership suggests about product fit or integration potential. 
+• Leverage: How to use that credibility to guide outreach. 
+Focus on leveraging the referral trust and highlighting integration or ecosystem relevance. 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Affiliates_TheTop10sites
-Engagement method: Referred through affiliate partner - has some context about RingCentral
-Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
-Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
-Secondary channel: Referred by direct affiliate - warm intro with initial context
-Specific engagement context: Affiliate referral - cost-per-lead, mid-intent form fill
-Target customer profile program classification: Ongoing evergreen campaign - continous lead flow
-Target customer profile and strategy: Targeting small business (1-499 employees) - faster sales cycle, price sensitive
+Engagement method: Affiliates: Referred through affiliate partner - has some context about RingCentral
+Cross channel marketing integration indicator: MVP/PBX to Cloud: Migration from on-premise focus - cost savings pitch
+Product interest: RingEX: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: Direct Affiliates: Referred by direct affiliate - warm intro with initial context
+Specific engagement context: Affiliates - CPL: Affiliate referral - cost-per-lead, mid-intent form fill
+Target customer profile program classification: Greenfield: Ongoing evergreen campaign - continous lead flow
+Target customer profile and strategy: RingEX SMB Acquisition: Targeting small business (1-499 employees) - faster sales cycle, price sensitive
 Lead source context: Better Impression (US)
-Company size segment: 20-99 employees - growing company, scalability important
+Company size segment: SMB: 20-99 employees - growing company, scalability important
 Buyer journey stage: High intent - actively evaluating solutions (demo, trial, pricing interest)
 Campaign description: Prospect visited RingCentral Office Landing Page from a Comparison/Review Website - TheTop10Sites.com (https://www.thetop10sites.com/business-voip/) and submitted their info through the web form or called in.
 Campaign title: Affiliates_TheTop10sites
@@ -1318,9 +1346,9 @@
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>• Referral Source: Trusted third-party referral from TheTop10Sites.com
-• Fit/Alignment: Implies strong product fit for UCaaS/business phone system
-• Leverage: Highlight partnership credibility, emphasize integration potential</t>
+          <t>• Referral Source: Referred via trusted affiliate partner TheTop10Sites.com
+• Fit/Alignment: Indicates interest in RingEX UCaaS for SMB, IT decision maker
+• Leverage: Highlight integration potential, mention referral for credibility</t>
         </is>
       </c>
     </row>
@@ -1404,19 +1432,23 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Referral Source: This lead came through a trusted third party referral or partner. • Fit/Alignment: What the partnership suggests about product fit or integration potential. • Leverage: How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Referral Source: This lead came through a trusted third party referral or partner. 
+• Fit/Alignment: What the partnership suggests about product fit or integration potential. 
+• Leverage: How to use that credibility to guide outreach. 
+Focus on leveraging the referral trust and highlighting integration or ecosystem relevance. 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Affiliates_BusinessBPS
-Engagement method: Referred through affiliate partner - has some context about RingCentral
-Cross channel marketing integration indicator: Migration from on-premise focus - cost savings pitch
-Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
-Secondary channel: Referred by direct affiliate - warm intro with initial context
-Specific engagement context: Clicked cost-per-click affiliate link - low-friction awareness
-Target customer profile program classification: Ongoing evergreen campaign - continous lead flow
-Target customer profile and strategy: Targeting small business (1-499 employees) - faster sales cycle, price sensitive
+Engagement method: Affiliates: Referred through affiliate partner - has some context about RingCentral
+Cross channel marketing integration indicator: MVP/PBX to Cloud: Migration from on-premise focus - cost savings pitch
+Product interest: RingEX: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: Direct Affiliates: Referred by direct affiliate - warm intro with initial context
+Specific engagement context: Affiliates - CPC: Clicked cost-per-click affiliate link - low-friction awareness
+Target customer profile program classification: Greenfield: Ongoing evergreen campaign - continous lead flow
+Target customer profile and strategy: RingEX SMB Acquisition: Targeting small business (1-499 employees) - faster sales cycle, price sensitive
 Lead source context: Purch (Business News Daily - VOIP)
-Company size segment: 20-99 employees - growing company, scalability important
+Company size segment: SMB: 20-99 employees - growing company, scalability important
 Buyer journey stage: High intent - actively evaluating solutions (demo, trial, pricing interest)
 Campaign description: Prospect visited RingCentral Office Landing Page from a Content/Review Website - Business.com (https://www.business.com/categories/business-phone-systems/) and submitted their info through the web form or called in.
 Campaign title: Affiliates_BusinessBPS
@@ -1428,9 +1460,9 @@
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>• Referral Source: Referred through trusted partner.
-• Fit/Alignment: Partnership indicates strong product fit.
-• Leverage: Highlight integration relevance, mention referral credibility.</t>
+          <t>- Referral Source: Trusted third party referral from Business.com - indicates interest in RingEX UCaaS
+- Fit/Alignment: Partnership suggests strong product fit or integration potential for RingCentral
+- Leverage: Use referral credibility to guide outreach with focus on integration benefits</t>
         </is>
       </c>
     </row>
@@ -1502,14 +1534,18 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Search Behavior: The lead actively searched for a solution or visited our site. • Trigger: What keyword or campaign may have triggered the engagement. • Urgency: How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Search Behavior: The lead actively searched for a solution or visited our site. 
+• Trigger: What keyword or campaign may have triggered the engagement. 
+• Urgency: How to tailor outreach based on urgency or solution comparison. 
+Focus on urgency, buyer readiness, and solution fit. 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Bing_US_Search_Brand_Exact
-Engagement method: Clicked on search ads - actively searching for communication solutions with high intent
-Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
-Secondary channel: Found via RingCentral brand keyword search - direct high intent query
-Specific engagement context: Searched 'RingCentral' or product names - brand aware, high intent
+Engagement method: Paid Search: Clicked on search ads - actively searching for communication solutions with high intent
+Product interest: RingEX: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: Brand Search: Found via RingCentral brand keyword search - direct high intent query
+Specific engagement context: SEM - Brand: Searched 'RingCentral' or product names - brand aware, high intent
 Lead source context: Bing
 Campaign description: Paid Search
 Campaign title: Bing_US_Search_Brand_Exact
@@ -1521,9 +1557,9 @@
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>• Search Behavior: Lead actively searched for communication solutions, visited RingCentral site
-• Trigger: Bing_US_Search_Brand_Exact campaign, RingCentral brand keyword search
-• Urgency: Tailor outreach for IT decision maker, high intent, compare solutions, emphasize UCaaS benefits</t>
+          <t>• Search Behavior: Lead actively searched for communication solutions, likely a tech-savvy IT decision maker interested in RingEX UCaaS.  
+• Trigger: Engaged via Bing_US_Search_Brand_Exact campaign, showing high intent through brand keyword search.  
+• Urgency: Tailor outreach addressing urgent UCaaS needs, emphasizing RingEX fit for seamless communication solutions.</t>
         </is>
       </c>
     </row>
@@ -1583,13 +1619,17 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Referral Source: This lead came through a trusted third party referral or partner. • Fit/Alignment: What the partnership suggests about product fit or integration potential. • Leverage: How to use that credibility to guide outreach. Focus on leveraging the referral trust and highlighting integration or ecosystem relevance.
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Referral Source: This lead came through a trusted third party referral or partner. 
+• Fit/Alignment: What the partnership suggests about product fit or integration potential. 
+• Leverage: How to use that credibility to guide outreach. 
+Focus on leveraging the referral trust and highlighting integration or ecosystem relevance. 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: RCO/ACO_Price_Parity
-Engagement method: Campaign funded through reseller marketing - likely co-branded outreach via trusted tech advisor
-Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
-Secondary channel: Event marketing - webinars, conferences, tradeshows
+Engagement method: VAR MDF: Campaign funded through reseller marketing - likely co-branded outreach via trusted tech advisor
+Product interest: RingEX: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: Events: Event marketing - webinars, conferences, tradeshows
 Lead source context: VAR Marketing
 Campaign title: RCO/ACO_Price_Parity
 Target geographic market for campaign: US
@@ -1599,9 +1639,9 @@
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>• Referral Source: Lead from trusted tech advisor
-• Fit/Alignment: Indicates strong fit for UCaaS solutions
-• Leverage: Highlight partnership credibility, emphasize integration potential for unified communications.</t>
+          <t>• Referral Source: Trusted tech advisor referred this lead, suggesting strong credibility and interest in RingEX UCaaS. 
+• Fit/Alignment: Partnership indicates potential for seamless integration, highlighting product fit for unified communications. 
+• Leverage: Emphasize the referral trust to position RingEX as a natural choice for their tech ecosystem.</t>
         </is>
       </c>
     </row>
@@ -1657,13 +1697,17 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Search Behavior: The lead actively searched for a solution or visited our site. • Trigger: What keyword or campaign may have triggered the engagement. • Urgency: How to tailor outreach based on urgency or solution comparison. Focus on urgency, buyer readiness, and solution fit.
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Search Behavior: The lead actively searched for a solution or visited our site. 
+• Trigger: What keyword or campaign may have triggered the engagement. 
+• Urgency: How to tailor outreach based on urgency or solution comparison. 
+Focus on urgency, buyer readiness, and solution fit. 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: SEO_GoogleRC
-Engagement method: Found us through organic search - self-directed research, comparing options
-Product interest: UCaaS/business phone system buyer - likely IT decision maker for unified communications
-Secondary channel: SEM/SEO driven - paid or organic search
+Engagement method: Organic Search: Found us through organic search - self-directed research, comparing options
+Product interest: RingEX: UCaaS/business phone system buyer - likely IT decision maker for unified communications
+Secondary channel: Search Engines: SEM/SEO driven - paid or organic search
 Campaign title: SEO_GoogleRC
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
@@ -1672,9 +1716,9 @@
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>• Search Behavior: Lead actively researching UCaaS options, found us through organic search.
-• Trigger: Likely searched keywords related to UCaaS or business phone systems.
-• Urgency: Tailor outreach based on solution readiness and immediate need for unified communications.</t>
+          <t>• Search Behavior: Lead actively searched for a UCaaS/business phone system solution or visited our site.
+• Trigger: Potential keyword triggers include "UCaaS providers" or "business phone systems comparison."
+• Urgency: Tailor outreach based on urgency for IT decision makers evaluating unified communications solutions.</t>
         </is>
       </c>
     </row>
@@ -1730,12 +1774,16 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Participation: The prospect attended a live event or self submitted interest. • Signal: What this action suggests about their current interest or goals. • Engagement Style: How to follow up in a relationship driven or consultative way. Focus on event context and tailoring outreach around shared experience or learning goals.
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Participation: The prospect attended a live event or self submitted interest. 
+• Signal: What this action suggests about their current interest or goals. 
+• Engagement Style: How to follow up in a relationship driven or consultative way. 
+Focus on event context and tailoring outreach around shared experience or learning goals. 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: Sales Generated
-Engagement method: Self-submitted or inbound lead without campaign - high initiative, potentially urgent need
-Secondary channel: Entered by sales team from internal source - low initial engagement
+Engagement method: Walk-On: Self-submitted or inbound lead without campaign - high initiative, potentially urgent need
+Secondary channel: Sales Generated: Entered by sales team from internal source - low initial engagement
 Campaign title: Sales Generated
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
@@ -1744,9 +1792,9 @@
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>• Participation: Prospect self-submitted interest for Sales Generated campaign. 
-• Signal: Shows high initiative and potential urgent need for sales solutions. 
-• Engagement Style: Follow up with a consultative approach, referencing shared learning goals from Sales Generated website.</t>
+          <t>• Participation: Prospects showed high initiative by self-submitting interest or attending an event related to our product. 
+• Signal: Indicates urgent need or strong interest in addressing specific challenges related to our product. 
+• Engagement Style: Follow up with a consultative approach, focusing on shared experiences or learning goals from the event.</t>
         </is>
       </c>
     </row>
@@ -1818,14 +1866,18 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Source: This is a sales-sourced contact (not from prospect engagement). • Data Origin: The data source and why this contact was identified. • Approach: What approach might work best for cold outreach. Focus on the sales context and potential fit, not prospect behavior (since they haven't engaged).
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Source: This is a sales-sourced contact (not from prospect engagement). 
+• Data Origin: The data source and why this contact was identified. 
+• Approach: What approach might work best for cold outreach. 
+Focus on the sales context and potential fit, not prospect behavior (since they haven't engaged). 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: HealthcareLPformfills
-Engagement method: Engagment channel not categorized - review needed to determine buyer intent
-Secondary channel: Direct website visit or form fill - proactive buyer behavior
+Engagement method: Other: Engagment channel not categorized - review needed to determine buyer intent
+Secondary channel: website: Direct website visit or form fill - proactive buyer behavior
 Lead source context: Healthcare
-Industry context: Healthcare industry - HIPAA compilance needs
+Industry context: Healthcare: Healthcare industry - HIPAA compilance needs
 Campaign description: Healthcare integrated campaign
 Campaign title: HealthcareLPformfills
 Target geographic market for campaign: US
@@ -1837,8 +1889,8 @@
       <c r="W14" t="inlineStr">
         <is>
           <t>• Source: Sales-sourced contact
-• Data Origin: Identified through HealthcareLPformfills campaign
-• Approach: Highlight HIPAA compliance benefits in cold outreach</t>
+• Data Origin: Identified from Healthcare industry context 
+• Approach: Personalized outreach highlighting healthcare product benefits</t>
         </is>
       </c>
     </row>
@@ -1894,12 +1946,16 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>Based on the following campaign information, help a salesperson understand (format as exactly 3 bullet points with the specified category labels, total 255 characters max): • Participation: The prospect attended a live event or self submitted interest. • Signal: What this action suggests about their current interest or goals. • Engagement Style: How to follow up in a relationship driven or consultative way. Focus on event context and tailoring outreach around shared experience or learning goals.
+          <t>You are generating a campaign description for a sales rep. Use the provided Salesforce campaign metadata to infer campaign purpose, prospect behavior, and recommended rep follow up. Output exactly 3 concise bullet points with the specified category labels: Descriptions should be clear, relevant, quick to read, and under 255 characters total. Always mention the product interest if it's available. DO NOT repeat the campaign name. Write with the goal of helping a sales rep understand the prospect's mindset and how to follow up: 
+• Participation: The prospect attended a live event or self submitted interest. 
+• Signal: What this action suggests about their current interest or goals. 
+• Engagement Style: How to follow up in a relationship driven or consultative way. 
+Focus on event context and tailoring outreach around shared experience or learning goals. 
 IMPORTANT: If the campaign details mention any URLs or websites, preserve the domain name in your description.
 Campaign Information:
 Campaign: True_Walk_On_2024
-Engagement method: Self-submitted or inbound lead without campaign - high initiative, potentially urgent need
-Secondary channel: Inbound lead without source - prospect found us directly
+Engagement method: Walk-On: Self-submitted or inbound lead without campaign - high initiative, potentially urgent need
+Secondary channel: Walk-On: Inbound lead without source - prospect found us directly
 Campaign title: True_Walk_On_2024
 Target geographic market for campaign: US
 Attribution tracking: Can clearly track that a lead came from this specific campaign (clear cause + effect)
@@ -1908,9 +1964,9 @@
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>• Participation: Prospect self-submitted interest for True_Walk_On_2024.
-• Signal: Indicates high initiative and potentially urgent need.
-• Engagement Style: Emphasize shared experience or learning goals in a consultative follow-up approach.</t>
+          <t>• Participation: Prospect self-submitted interest or found us directly without source.
+• Signal: Indicates high initiative and potentially urgent need related to our product.
+• Engagement Style: Follow up in a consultative manner, acknowledging their proactive approach and addressing their urgent needs.</t>
         </is>
       </c>
     </row>
@@ -2009,7 +2065,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>248.6 chars</t>
+          <t>307.3 chars</t>
         </is>
       </c>
     </row>
@@ -2030,7 +2086,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.37</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -2111,7 +2167,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-07-21 13:55:37</t>
+          <t>2025-07-22 12:39:42</t>
         </is>
       </c>
     </row>

</xml_diff>